<commit_message>
Updated Electrolysis Technologies, Germany Data for Trade Route & updated  values for GrowthRateTradeCap
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v05_joh_19-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v05_joh_19-09-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dozeumhaj\Documents\GENeSYS_MOD.data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5DA799-2C8E-4058-A387-3258C44DF2AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0A92D0-5909-455B-B0E0-2334BE45C0FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="8" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -1256,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,90 +1599,144 @@
       <c r="A42" t="s">
         <v>263</v>
       </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>264</v>
       </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>265</v>
       </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>266</v>
       </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>267</v>
       </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>268</v>
       </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>280</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3599,7 +3653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D817F8-1014-4E28-A827-54661E8BA006}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F25:F26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Data update for Germany
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v05_joh_19-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v05_joh_19-09-2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dozeumhaj\Documents\GENeSYS_MOD.data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0A92D0-5909-455B-B0E0-2334BE45C0FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC2C45C-4216-4BDE-B19B-60D6D96EB61E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
@@ -1256,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41:B59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,7 +1360,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1368,7 +1368,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1376,7 +1376,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1384,7 +1384,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1392,7 +1392,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1416,7 +1416,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1440,7 +1440,7 @@
         <v>19</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
         <v>20</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1456,7 +1456,7 @@
         <v>21</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
         <v>23</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
         <v>24</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1488,7 +1488,7 @@
         <v>25</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1496,7 +1496,7 @@
         <v>26</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>27</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1512,7 +1512,7 @@
         <v>28</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1520,7 +1520,7 @@
         <v>3</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
         <v>29</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1536,7 +1536,7 @@
         <v>30</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1544,7 +1544,7 @@
         <v>31</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
         <v>32</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1560,7 +1560,7 @@
         <v>33</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1568,7 +1568,7 @@
         <v>34</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
         <v>35</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1584,7 +1584,7 @@
         <v>36</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1592,7 +1592,7 @@
         <v>37</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>